<commit_message>
Ajustes para incluir más M101A en consolidación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="230">
   <si>
     <t>Asignatura</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>Actividad que sirve para reforzar la comprensión de la relación entre los tipos de neuronas y la función que desempeñan</t>
+  </si>
+  <si>
+    <t>Recurso M101A-03</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3242,7 +3245,7 @@
         <v>146</v>
       </c>
       <c r="T26" s="57" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="U26" s="56" t="s">
         <v>148</v>
@@ -3301,7 +3304,7 @@
         <v>146</v>
       </c>
       <c r="T27" s="57" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="U27" s="56" t="s">
         <v>148</v>
@@ -3580,11 +3583,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3600,6 +3598,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Escaleta con columna a la izquierda
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -826,7 +826,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1178,12 +1178,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1373,9 +1399,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1413,6 +1436,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1688,7 +1717,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1698,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,8 +1745,8 @@
     <col min="10" max="10" width="92.28515625" style="18" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="40" customWidth="1"/>
-    <col min="14" max="14" width="5" style="18" customWidth="1"/>
+    <col min="13" max="13" width="5" style="18" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="40" customWidth="1"/>
     <col min="15" max="15" width="60" style="41" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" style="24" customWidth="1"/>
     <col min="17" max="17" width="7.28515625" style="18" customWidth="1"/>
@@ -1759,20 +1788,20 @@
       <c r="J1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="67"/>
+      <c r="N1" s="81"/>
       <c r="O1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="68" t="s">
         <v>13</v>
       </c>
       <c r="Q1" s="65" t="s">
@@ -1802,21 +1831,21 @@
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
       <c r="J2" s="66"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="23" t="s">
-        <v>87</v>
-      </c>
       <c r="O2" s="66"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -1851,10 +1880,10 @@
       <c r="L3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33" t="s">
+      <c r="M3" s="33" t="s">
         <v>35</v>
       </c>
+      <c r="N3" s="33"/>
       <c r="O3" s="63" t="s">
         <v>159</v>
       </c>
@@ -1912,10 +1941,10 @@
       <c r="L4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="16"/>
       <c r="O4" s="17" t="s">
         <v>160</v>
       </c>
@@ -1975,10 +2004,10 @@
       <c r="L5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>40</v>
       </c>
+      <c r="N5" s="16"/>
       <c r="O5" s="17" t="s">
         <v>164</v>
       </c>
@@ -2038,10 +2067,10 @@
       <c r="L6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
+      <c r="M6" s="16" t="s">
         <v>44</v>
       </c>
+      <c r="N6" s="16"/>
       <c r="O6" s="15" t="s">
         <v>165</v>
       </c>
@@ -2101,10 +2130,10 @@
       <c r="L7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="16"/>
+      <c r="N7" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="16"/>
       <c r="O7" s="17"/>
       <c r="P7" s="37" t="s">
         <v>19</v>
@@ -2162,10 +2191,10 @@
       <c r="L8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16" t="s">
+      <c r="M8" s="16" t="s">
         <v>36</v>
       </c>
+      <c r="N8" s="16"/>
       <c r="O8" s="15" t="s">
         <v>169</v>
       </c>
@@ -2225,10 +2254,10 @@
       <c r="L9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="N9" s="16"/>
       <c r="O9" s="17"/>
       <c r="P9" s="37" t="s">
         <v>19</v>
@@ -2286,10 +2315,10 @@
       <c r="L10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="16"/>
+      <c r="N10" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="16"/>
       <c r="O10" s="17"/>
       <c r="P10" s="37" t="s">
         <v>20</v>
@@ -2347,10 +2376,10 @@
       <c r="L11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="16"/>
+      <c r="N11" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="16"/>
       <c r="O11" s="17"/>
       <c r="P11" s="37" t="s">
         <v>19</v>
@@ -2463,10 +2492,10 @@
       <c r="L13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16" t="s">
+      <c r="M13" s="16" t="s">
         <v>41</v>
       </c>
+      <c r="N13" s="16"/>
       <c r="O13" s="17"/>
       <c r="P13" s="37" t="s">
         <v>19</v>
@@ -2522,10 +2551,10 @@
       <c r="L14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16" t="s">
+      <c r="M14" s="16" t="s">
         <v>35</v>
       </c>
+      <c r="N14" s="16"/>
       <c r="O14" s="15" t="s">
         <v>173</v>
       </c>
@@ -2583,10 +2612,10 @@
       <c r="L15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="16"/>
+      <c r="N15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="N15" s="16"/>
       <c r="O15" s="15"/>
       <c r="P15" s="37" t="s">
         <v>20</v>
@@ -2642,10 +2671,10 @@
       <c r="L16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="16"/>
+      <c r="N16" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="16"/>
       <c r="O16" s="15" t="s">
         <v>221</v>
       </c>
@@ -2701,10 +2730,10 @@
       <c r="L17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16" t="s">
+      <c r="M17" s="16" t="s">
         <v>36</v>
       </c>
+      <c r="N17" s="16"/>
       <c r="O17" s="15" t="s">
         <v>183</v>
       </c>
@@ -2760,10 +2789,10 @@
       <c r="L18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="16"/>
+      <c r="N18" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="N18" s="16"/>
       <c r="O18" s="17"/>
       <c r="P18" s="37" t="s">
         <v>19</v>
@@ -2988,10 +3017,10 @@
       <c r="L22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16" t="s">
+      <c r="M22" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="N22" s="16"/>
       <c r="O22" s="15" t="s">
         <v>189</v>
       </c>
@@ -3049,10 +3078,10 @@
       <c r="L23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="16" t="s">
+      <c r="M23" s="16"/>
+      <c r="N23" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N23" s="16"/>
       <c r="O23" s="15" t="s">
         <v>191</v>
       </c>
@@ -3110,10 +3139,10 @@
       <c r="L24" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="16"/>
+      <c r="N24" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="16"/>
       <c r="O24" s="15" t="s">
         <v>197</v>
       </c>
@@ -3171,10 +3200,10 @@
       <c r="L25" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="16"/>
+      <c r="N25" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N25" s="16"/>
       <c r="O25" s="15" t="s">
         <v>201</v>
       </c>
@@ -3232,10 +3261,10 @@
       <c r="L26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M26" s="16" t="s">
+      <c r="M26" s="16"/>
+      <c r="N26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="N26" s="16"/>
       <c r="O26" s="15" t="s">
         <v>196</v>
       </c>
@@ -3293,10 +3322,10 @@
       <c r="L27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="64" t="s">
+      <c r="M27" s="16"/>
+      <c r="N27" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="N27" s="16"/>
       <c r="O27" s="15" t="s">
         <v>202</v>
       </c>
@@ -3507,10 +3536,10 @@
       <c r="L31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="16" t="s">
+      <c r="M31" s="16"/>
+      <c r="N31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="16"/>
       <c r="O31" s="17"/>
       <c r="P31" s="37" t="s">
         <v>19</v>
@@ -3564,10 +3593,10 @@
       <c r="L32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M32" s="16" t="s">
+      <c r="M32" s="16"/>
+      <c r="N32" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="N32" s="16"/>
       <c r="O32" s="17"/>
       <c r="P32" s="37" t="s">
         <v>20</v>
@@ -3590,11 +3619,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3610,6 +3634,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3644,13 +3673,13 @@
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M32</xm:sqref>
+          <xm:sqref>N3:N32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N32</xm:sqref>
+          <xm:sqref>M3:M32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4324,40 +4353,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="74" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="76"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="75"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">

</xml_diff>

<commit_message>
Cambios en videos y audios
Se eliminan las peticiones de audios y videos nuevos, y se agregan las
solicitudes de videos (incompletas. Falta matrícula del video)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="VER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -368,9 +368,6 @@
     <t>Actividad que permite repasar las diferencias estructurales y funcionales entre el sistema nervioso central y el periférico</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: el sistema nervioso </t>
-  </si>
-  <si>
     <t>Actividades sobre el sistema nervioso</t>
   </si>
   <si>
@@ -389,9 +386,6 @@
     <t>Alteraciones por enfermedades</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: las alteraciones del sistema nervioso</t>
-  </si>
-  <si>
     <t>Actividad sobre las alteraciones del sistema nervioso</t>
   </si>
   <si>
@@ -494,9 +488,6 @@
     <t>Interactivo que explora la función y la importancia del sistema nervioso</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: las reacciones al entorno</t>
-  </si>
-  <si>
     <t>Actividad para consolidar los aprendido sobre la respuesta al entorno que posibilita el sistema nervioso</t>
   </si>
   <si>
@@ -518,9 +509,6 @@
     <t xml:space="preserve">Sobre la imagen de una neurona se señalas el cuerpo neuronal o soma, las dendritas, y el axón. </t>
   </si>
   <si>
-    <t>Se anima la formación y transmisión de impulsos nerviosos por cambios en la concentración de iones a cada lado de la membrana celular</t>
-  </si>
-  <si>
     <t>El funcionamiento de las neuronas</t>
   </si>
   <si>
@@ -545,9 +533,6 @@
     <t xml:space="preserve">Se presentan las células gliales y la mielina, y se explica su función dentro del sistema nervioso (proteger y aislar eléctricamente las neuronas). Antes de abordar diversos aspectos, se cuestiona a los estudianes qué crreen sobre cada uno (por ejemplo, ¿todas las neuornas están cubiertas por células gliales? Ahí se explica que dichas ce´luals no recubren todas las neuronas, se dice en donde sí están etc.) </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la estructura del sistema nervioso</t>
-  </si>
-  <si>
     <t>Actividad para consolidar lo aprendido acerca de la estructura del sistema nervioso</t>
   </si>
   <si>
@@ -614,9 +599,6 @@
     <t>Se presentan diversas opciones de alteraciones (infección vírica, por ejemplo) para que el estudiante la ubique en el contenedor correcto: alteraciones por causas físicas, alteraciones por causas químicas, alteraciones por enfermedades y alteraciones por otras causas.</t>
   </si>
   <si>
-    <t xml:space="preserve">Se hace un texto que hable sobre causas qu´micas de alteraciones: falta de nutrientes por desnutrición, intoxicación por productos químicos, adicción a las drogas, etc. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para reforzar la comprensión de las causas de alteración del sistema nervioso </t>
   </si>
   <si>
@@ -641,9 +623,6 @@
     <t>Recurso F8-01</t>
   </si>
   <si>
-    <t>Recurso F12-01</t>
-  </si>
-  <si>
     <t>Recurso F6-01</t>
   </si>
   <si>
@@ -714,6 +693,27 @@
   </si>
   <si>
     <t>Motor que incluye preguntas de respuesta abierta del tema El sistema nervioso</t>
+  </si>
+  <si>
+    <t>Se hace un texto que hable sobre causas químicas de alteraciones: falta de nutrientes por desnutrición, intoxicación por productos químicos, adicción a las drogas, etc.</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las reacciones al entorno</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La estructura del sistema nervioso</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las alteraciones del sistema nervioso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: El sistema nervioso </t>
+  </si>
+  <si>
+    <t>Se ilustra la formación y transmisión de impulsos nerviosos por cambios en la concentración de iones a cada lado de la membrana celular. Como este es un proceso comlplejo, se divide en pasos que se van mostrando en cada pestaña. Aprovechar las pestañas de más información para explicar procesos y aclarar términos como diferencia de potencial o iones. Las preguntas consolidación la comprensión del estado d elas cosas en cada momento. Por ejemplo, si hay una diferencia de potencial de manera que el interior de la membrana es más negativo que el exterior, ¿hacia dónde se moverán los cationes si los canales de la membrana se abren? Las respuestas serían "Al interior de la célula" o "Al exterior de la célula".</t>
+  </si>
+  <si>
+    <t>Recurso F4-03</t>
   </si>
 </sst>
 </file>
@@ -1399,6 +1399,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1436,12 +1442,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1717,7 +1717,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1727,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,20 +1788,20 @@
       <c r="J1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="M1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="81"/>
+      <c r="N1" s="68"/>
       <c r="O1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="68" t="s">
+      <c r="P1" s="70" t="s">
         <v>13</v>
       </c>
       <c r="Q1" s="65" t="s">
@@ -1831,8 +1831,8 @@
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
       <c r="J2" s="66"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="69"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="71"/>
       <c r="M2" s="23" t="s">
         <v>87</v>
       </c>
@@ -1840,12 +1840,12 @@
         <v>86</v>
       </c>
       <c r="O2" s="66"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -1872,7 +1872,7 @@
         <v>103</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K3" s="31" t="s">
         <v>69</v>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P3" s="34" t="s">
         <v>19</v>
@@ -1894,16 +1894,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="50" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S3" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="U3" s="52" t="s">
         <v>152</v>
-      </c>
-      <c r="T3" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="U3" s="52" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>157</v>
+        <v>225</v>
       </c>
       <c r="H4" s="13">
         <v>2</v>
@@ -1933,7 +1933,7 @@
         <v>94</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>69</v>
@@ -1946,7 +1946,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P4" s="37" t="s">
         <v>19</v>
@@ -1955,19 +1955,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S4" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="U4" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="T4" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="U4" s="56" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>67</v>
       </c>
@@ -1984,10 +1984,10 @@
         <v>101</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H5" s="13">
         <v>3</v>
@@ -1996,7 +1996,7 @@
         <v>103</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>69</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="P5" s="37" t="s">
         <v>19</v>
@@ -2018,16 +2018,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S5" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="T5" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="U5" s="56" t="s">
         <v>152</v>
-      </c>
-      <c r="T5" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="U5" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
         <v>101</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>102</v>
@@ -2059,38 +2059,38 @@
         <v>103</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="15" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="P6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="53">
+      <c r="Q6" s="49">
         <v>6</v>
       </c>
-      <c r="R6" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="S6" s="54" t="s">
+      <c r="R6" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="S6" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="T6" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="U6" s="52" t="s">
         <v>152</v>
-      </c>
-      <c r="T6" s="55" t="s">
-        <v>206</v>
-      </c>
-      <c r="U6" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2110,10 +2110,10 @@
         <v>101</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H7" s="13">
         <v>5</v>
@@ -2122,7 +2122,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>69</v>
@@ -2142,16 +2142,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="S7" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T7" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="54" t="s">
+      <c r="U7" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T7" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="U7" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>104</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H8" s="13">
         <v>6</v>
@@ -2183,7 +2183,7 @@
         <v>103</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>69</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="N8" s="16"/>
       <c r="O8" s="15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P8" s="37" t="s">
         <v>19</v>
@@ -2205,16 +2205,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S8" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="T8" s="55" t="s">
+        <v>200</v>
+      </c>
+      <c r="U8" s="56" t="s">
         <v>152</v>
-      </c>
-      <c r="T8" s="55" t="s">
-        <v>207</v>
-      </c>
-      <c r="U8" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
         <v>104</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H9" s="13">
         <v>7</v>
@@ -2246,7 +2246,7 @@
         <v>103</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>69</v>
@@ -2266,16 +2266,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="S9" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="T9" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="S9" s="59" t="s">
+      <c r="U9" s="61" t="s">
         <v>152</v>
-      </c>
-      <c r="T9" s="60" t="s">
-        <v>153</v>
-      </c>
-      <c r="U9" s="61" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
         <v>104</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H10" s="13">
         <v>8</v>
@@ -2307,7 +2307,7 @@
         <v>94</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>69</v>
@@ -2327,16 +2327,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S10" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T10" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="U10" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T10" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="U10" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>104</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H11" s="13">
         <v>9</v>
@@ -2368,7 +2368,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>69</v>
@@ -2388,16 +2388,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S11" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T11" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="U11" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T11" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="U11" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H12" s="13">
         <v>10</v>
@@ -2427,7 +2427,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>70</v>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H13" s="13">
         <v>11</v>
@@ -2484,7 +2484,7 @@
         <v>103</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>69</v>
@@ -2504,16 +2504,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="59" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S13" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="T13" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="U13" s="61" t="s">
         <v>152</v>
-      </c>
-      <c r="T13" s="60" t="s">
-        <v>155</v>
-      </c>
-      <c r="U13" s="61" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>103</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>69</v>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="N14" s="16"/>
       <c r="O14" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="P14" s="37" t="s">
         <v>19</v>
@@ -2565,16 +2565,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="59" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S14" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="T14" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="U14" s="61" t="s">
         <v>152</v>
-      </c>
-      <c r="T14" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="U14" s="61" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H15" s="13">
         <v>13</v>
@@ -2604,7 +2604,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>69</v>
@@ -2624,16 +2624,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S15" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T15" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="U15" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T15" s="57" t="s">
-        <v>150</v>
-      </c>
-      <c r="U15" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="12" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="H16" s="13">
         <v>14</v>
@@ -2663,7 +2663,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>69</v>
@@ -2676,7 +2676,7 @@
         <v>62</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="P16" s="37" t="s">
         <v>19</v>
@@ -2685,16 +2685,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S16" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T16" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="U16" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T16" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="U16" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2708,12 +2708,12 @@
         <v>91</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="38"/>
       <c r="G17" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2722,7 +2722,7 @@
         <v>103</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>69</v>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="15" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="P17" s="37" t="s">
         <v>19</v>
@@ -2744,16 +2744,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S17" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="T17" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="U17" s="56" t="s">
         <v>152</v>
-      </c>
-      <c r="T17" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="U17" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2767,12 +2767,12 @@
         <v>91</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="38"/>
       <c r="G18" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H18" s="13">
         <v>16</v>
@@ -2781,7 +2781,7 @@
         <v>94</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>69</v>
@@ -2801,16 +2801,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S18" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T18" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="U18" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T18" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="U18" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <v>91</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>109</v>
@@ -2881,7 +2881,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>112</v>
@@ -2938,14 +2938,14 @@
         <v>91</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>99</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="12" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
       <c r="H21" s="13">
         <v>19</v>
@@ -2954,7 +2954,7 @@
         <v>94</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>70</v>
@@ -2978,7 +2978,7 @@
         <v>97</v>
       </c>
       <c r="T21" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U21" s="56" t="s">
         <v>98</v>
@@ -2995,12 +2995,12 @@
         <v>91</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
       <c r="G22" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H22" s="13">
         <v>20</v>
@@ -3009,7 +3009,7 @@
         <v>103</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>69</v>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="N22" s="16"/>
       <c r="O22" s="15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="P22" s="37" t="s">
         <v>19</v>
@@ -3031,16 +3031,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S22" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="T22" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="U22" s="56" t="s">
         <v>152</v>
-      </c>
-      <c r="T22" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="U22" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -3054,14 +3054,14 @@
         <v>91</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -3070,7 +3070,7 @@
         <v>94</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K23" s="14" t="s">
         <v>69</v>
@@ -3083,25 +3083,25 @@
         <v>84</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="P23" s="37" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Q23" s="53">
         <v>6</v>
       </c>
       <c r="R23" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S23" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T23" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="U23" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T23" s="57" t="s">
-        <v>211</v>
-      </c>
-      <c r="U23" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -3115,14 +3115,14 @@
         <v>91</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H24" s="13">
         <v>22</v>
@@ -3131,7 +3131,7 @@
         <v>94</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>69</v>
@@ -3144,7 +3144,7 @@
         <v>77</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="P24" s="37" t="s">
         <v>19</v>
@@ -3153,16 +3153,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S24" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T24" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="U24" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T24" s="57" t="s">
-        <v>212</v>
-      </c>
-      <c r="U24" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -3176,14 +3176,14 @@
         <v>91</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H25" s="13">
         <v>23</v>
@@ -3192,7 +3192,7 @@
         <v>94</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>69</v>
@@ -3205,7 +3205,7 @@
         <v>84</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="P25" s="37" t="s">
         <v>19</v>
@@ -3214,16 +3214,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S25" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T25" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="U25" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T25" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="U25" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3237,14 +3237,14 @@
         <v>91</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="12" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H26" s="13">
         <v>24</v>
@@ -3253,7 +3253,7 @@
         <v>94</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K26" s="14" t="s">
         <v>69</v>
@@ -3266,7 +3266,7 @@
         <v>24</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="P26" s="37" t="s">
         <v>19</v>
@@ -3275,16 +3275,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S26" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T26" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="U26" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T26" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="U26" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3298,14 +3298,14 @@
         <v>91</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="12" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="H27" s="13">
         <v>25</v>
@@ -3314,7 +3314,7 @@
         <v>94</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>69</v>
@@ -3327,7 +3327,7 @@
         <v>62</v>
       </c>
       <c r="O27" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="P27" s="37" t="s">
         <v>19</v>
@@ -3336,16 +3336,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S27" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T27" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="U27" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T27" s="57" t="s">
-        <v>216</v>
-      </c>
-      <c r="U27" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3359,12 +3359,12 @@
         <v>91</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
       <c r="G28" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H28" s="13">
         <v>26</v>
@@ -3373,7 +3373,7 @@
         <v>94</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>70</v>
@@ -3397,7 +3397,7 @@
         <v>97</v>
       </c>
       <c r="T28" s="55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U28" s="56" t="s">
         <v>98</v>
@@ -3414,12 +3414,12 @@
         <v>91</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -3428,7 +3428,7 @@
         <v>94</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K29" s="14" t="s">
         <v>70</v>
@@ -3452,7 +3452,7 @@
         <v>97</v>
       </c>
       <c r="T29" s="55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U29" s="56" t="s">
         <v>98</v>
@@ -3469,12 +3469,12 @@
         <v>91</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -3483,7 +3483,7 @@
         <v>94</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>69</v>
@@ -3514,12 +3514,12 @@
         <v>91</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -3528,7 +3528,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>69</v>
@@ -3548,16 +3548,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S31" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T31" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="U31" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T31" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="U31" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -3571,12 +3571,12 @@
         <v>91</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="12" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="H32" s="13">
         <v>30</v>
@@ -3585,7 +3585,7 @@
         <v>94</v>
       </c>
       <c r="J32" s="36" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>69</v>
@@ -3605,20 +3605,25 @@
         <v>6</v>
       </c>
       <c r="R32" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S32" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T32" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="U32" s="56" t="s">
         <v>143</v>
-      </c>
-      <c r="T32" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="U32" s="56" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3634,11 +3639,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4353,40 +4353,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="76" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="75"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H3" s="43"/>
     </row>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H4" s="43"/>
     </row>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H5" s="43"/>
     </row>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H6" s="43"/>
     </row>
@@ -4494,7 +4494,7 @@
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H7" s="43"/>
     </row>
@@ -4516,10 +4516,10 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="44" t="s">
         <v>139</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4540,10 +4540,10 @@
       </c>
       <c r="F9" s="46"/>
       <c r="G9" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H9" s="48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusión de proyectos método científico
Se modifican escaletas y guiones de octavo y noveno
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="234">
   <si>
     <t>Asignatura</t>
   </si>
@@ -714,6 +714,15 @@
   </si>
   <si>
     <t>Recurso F4-03</t>
+  </si>
+  <si>
+    <t>Competencias: plantear hipótesis en un experimento</t>
+  </si>
+  <si>
+    <t>Proyecto para generar preguntas e hipótesis en un experimento científico</t>
+  </si>
+  <si>
+    <t>Recurso F13-02</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -3469,12 +3478,12 @@
         <v>91</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="12" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -3483,25 +3492,37 @@
         <v>94</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>69</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="N30" s="16"/>
       <c r="O30" s="17"/>
       <c r="P30" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="55"/>
-      <c r="U30" s="56"/>
+        <v>20</v>
+      </c>
+      <c r="Q30" s="53">
+        <v>6</v>
+      </c>
+      <c r="R30" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="S30" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="T30" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="U30" s="56" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -3519,7 +3540,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -3528,37 +3549,25 @@
         <v>94</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>219</v>
+        <v>130</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>69</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M31" s="16"/>
-      <c r="N31" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="N31" s="16"/>
       <c r="O31" s="17"/>
       <c r="P31" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="53">
-        <v>6</v>
-      </c>
-      <c r="R31" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="S31" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="T31" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="U31" s="56" t="s">
-        <v>143</v>
-      </c>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="55"/>
+      <c r="U31" s="56"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
@@ -3576,7 +3585,7 @@
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="12" t="s">
-        <v>222</v>
+        <v>131</v>
       </c>
       <c r="H32" s="13">
         <v>30</v>
@@ -3585,7 +3594,7 @@
         <v>94</v>
       </c>
       <c r="J32" s="36" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>69</v>
@@ -3595,11 +3604,11 @@
       </c>
       <c r="M32" s="16"/>
       <c r="N32" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="O32" s="17"/>
       <c r="P32" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q32" s="53">
         <v>6</v>
@@ -3611,9 +3620,66 @@
         <v>141</v>
       </c>
       <c r="T32" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="U32" s="56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="H33" s="13">
+        <v>31</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O33" s="17"/>
+      <c r="P33" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="53">
+        <v>6</v>
+      </c>
+      <c r="R33" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="S33" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="T33" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="U32" s="56" t="s">
+      <c r="U33" s="56" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3649,37 +3715,37 @@
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A32</xm:sqref>
+          <xm:sqref>A3:A33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K32</xm:sqref>
+          <xm:sqref>K3:K33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L32</xm:sqref>
+          <xm:sqref>L3:L33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P32</xm:sqref>
+          <xm:sqref>P3:P33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N32</xm:sqref>
+          <xm:sqref>N3:N33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M32</xm:sqref>
+          <xm:sqref>M3:M33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Ajustes por cambios en escaleta
Numeración vieja
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20730" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="ESCALETA" sheetId="1" r:id="rId1"/>
     <sheet name="DATOS" sheetId="2" r:id="rId2"/>
     <sheet name="VER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="241">
   <si>
     <t>Asignatura</t>
   </si>
@@ -738,6 +738,12 @@
   </si>
   <si>
     <t>Recurso F6-03</t>
+  </si>
+  <si>
+    <t>Unir los tres tipos de neurona con la explicación de su función</t>
+  </si>
+  <si>
+    <t>Adaptar texto de fijación de recuerdos</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1748,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2285,9 @@
       <c r="N9" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="O9" s="16"/>
+      <c r="O9" s="14" t="s">
+        <v>239</v>
+      </c>
       <c r="P9" s="36" t="s">
         <v>20</v>
       </c>
@@ -2521,7 +2529,9 @@
         <v>41</v>
       </c>
       <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
+      <c r="O13" s="14" t="s">
+        <v>240</v>
+      </c>
       <c r="P13" s="36" t="s">
         <v>19</v>
       </c>
@@ -3762,6 +3772,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3777,11 +3792,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de nombre de rec110.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="20730" windowHeight="11640"/>
   </bookViews>
@@ -521,9 +526,6 @@
     <t>La transmisión de información entre células distintas</t>
   </si>
   <si>
-    <t>Interactivo que trata sobre la fijación de recuerdos en el sistema nervioso</t>
-  </si>
-  <si>
     <t>Interactivo acerca de las células gliales</t>
   </si>
   <si>
@@ -659,9 +661,6 @@
     <t>Las causas de alteración del sistema nervioso</t>
   </si>
   <si>
-    <t>Las conexiones neuronales y la memoria</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comprende como está organizado el sistema nervioso </t>
   </si>
   <si>
@@ -744,6 +743,12 @@
   </si>
   <si>
     <t>Adaptar texto de fijación de recuerdos</t>
+  </si>
+  <si>
+    <t>La plasticidad sináptica</t>
+  </si>
+  <si>
+    <t>Interactivo que trata sobre la plasticidad sináptica y su relación con los procesos cognitivos</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1755,7 +1760,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1932,7 @@
         <v>150</v>
       </c>
       <c r="T3" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U3" s="50" t="s">
         <v>151</v>
@@ -1951,7 +1956,7 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H4" s="12">
         <v>2</v>
@@ -1988,7 +1993,7 @@
         <v>141</v>
       </c>
       <c r="T4" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U4" s="54" t="s">
         <v>143</v>
@@ -2051,7 +2056,7 @@
         <v>150</v>
       </c>
       <c r="T5" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U5" s="54" t="s">
         <v>151</v>
@@ -2099,7 +2104,7 @@
       </c>
       <c r="N6" s="15"/>
       <c r="O6" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P6" s="36" t="s">
         <v>19</v>
@@ -2114,7 +2119,7 @@
         <v>150</v>
       </c>
       <c r="T6" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U6" s="50" t="s">
         <v>151</v>
@@ -2140,7 +2145,7 @@
         <v>161</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H7" s="12">
         <v>5</v>
@@ -2149,7 +2154,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>69</v>
@@ -2238,7 +2243,7 @@
         <v>150</v>
       </c>
       <c r="T8" s="53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U8" s="54" t="s">
         <v>151</v>
@@ -2264,7 +2269,7 @@
         <v>104</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H9" s="12">
         <v>7</v>
@@ -2273,7 +2278,7 @@
         <v>94</v>
       </c>
       <c r="J9" s="63" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>69</v>
@@ -2286,7 +2291,7 @@
         <v>74</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P9" s="36" t="s">
         <v>20</v>
@@ -2327,7 +2332,7 @@
         <v>104</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H10" s="12">
         <v>8</v>
@@ -2336,7 +2341,7 @@
         <v>103</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>69</v>
@@ -2349,7 +2354,7 @@
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P10" s="36" t="s">
         <v>19</v>
@@ -2364,7 +2369,7 @@
         <v>150</v>
       </c>
       <c r="T10" s="55" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="U10" s="54" t="s">
         <v>151</v>
@@ -2390,7 +2395,7 @@
         <v>104</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H11" s="12">
         <v>9</v>
@@ -2399,7 +2404,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>69</v>
@@ -2412,7 +2417,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P11" s="36" t="s">
         <v>19</v>
@@ -2427,7 +2432,7 @@
         <v>141</v>
       </c>
       <c r="T11" s="55" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="U11" s="54" t="s">
         <v>143</v>
@@ -2460,7 +2465,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>70</v>
@@ -2508,7 +2513,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="11" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="H13" s="12">
         <v>11</v>
@@ -2517,7 +2522,7 @@
         <v>103</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>69</v>
@@ -2530,7 +2535,7 @@
       </c>
       <c r="N13" s="15"/>
       <c r="O13" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="P13" s="36" t="s">
         <v>19</v>
@@ -2578,7 +2583,7 @@
         <v>103</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>69</v>
@@ -2591,7 +2596,7 @@
       </c>
       <c r="N14" s="15"/>
       <c r="O14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P14" s="36" t="s">
         <v>19</v>
@@ -2606,7 +2611,7 @@
         <v>150</v>
       </c>
       <c r="T14" s="58" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="U14" s="59" t="s">
         <v>151</v>
@@ -2630,7 +2635,7 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H15" s="12">
         <v>13</v>
@@ -2639,7 +2644,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>69</v>
@@ -2691,7 +2696,7 @@
         <v>104</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H16" s="12">
         <v>14</v>
@@ -2700,7 +2705,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>69</v>
@@ -2750,7 +2755,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H17" s="12">
         <v>15</v>
@@ -2759,7 +2764,7 @@
         <v>94</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>69</v>
@@ -2772,7 +2777,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P17" s="36" t="s">
         <v>19</v>
@@ -2787,7 +2792,7 @@
         <v>141</v>
       </c>
       <c r="T17" s="55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U17" s="54" t="s">
         <v>143</v>
@@ -2804,12 +2809,12 @@
         <v>91</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="37"/>
       <c r="G18" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H18" s="12">
         <v>16</v>
@@ -2818,7 +2823,7 @@
         <v>103</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>69</v>
@@ -2831,7 +2836,7 @@
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P18" s="36" t="s">
         <v>19</v>
@@ -2846,7 +2851,7 @@
         <v>150</v>
       </c>
       <c r="T18" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U18" s="54" t="s">
         <v>151</v>
@@ -2863,12 +2868,12 @@
         <v>91</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="37"/>
       <c r="G19" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H19" s="12">
         <v>17</v>
@@ -2877,7 +2882,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>69</v>
@@ -2920,7 +2925,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>109</v>
@@ -2977,7 +2982,7 @@
         <v>91</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>112</v>
@@ -3034,14 +3039,14 @@
         <v>91</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>99</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H22" s="12">
         <v>20</v>
@@ -3096,7 +3101,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H23" s="12">
         <v>21</v>
@@ -3105,7 +3110,7 @@
         <v>103</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K23" s="13" t="s">
         <v>69</v>
@@ -3118,7 +3123,7 @@
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P23" s="36" t="s">
         <v>19</v>
@@ -3133,7 +3138,7 @@
         <v>150</v>
       </c>
       <c r="T23" s="55" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="U23" s="54" t="s">
         <v>151</v>
@@ -3157,7 +3162,7 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H24" s="12">
         <v>22</v>
@@ -3166,7 +3171,7 @@
         <v>94</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>69</v>
@@ -3179,10 +3184,10 @@
         <v>84</v>
       </c>
       <c r="O24" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="P24" s="36" t="s">
         <v>182</v>
-      </c>
-      <c r="P24" s="36" t="s">
-        <v>183</v>
       </c>
       <c r="Q24" s="51">
         <v>6</v>
@@ -3194,7 +3199,7 @@
         <v>141</v>
       </c>
       <c r="T24" s="55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U24" s="54" t="s">
         <v>143</v>
@@ -3218,7 +3223,7 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H25" s="12">
         <v>23</v>
@@ -3227,7 +3232,7 @@
         <v>94</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>69</v>
@@ -3240,7 +3245,7 @@
         <v>77</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P25" s="36" t="s">
         <v>19</v>
@@ -3255,7 +3260,7 @@
         <v>141</v>
       </c>
       <c r="T25" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U25" s="54" t="s">
         <v>143</v>
@@ -3279,7 +3284,7 @@
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H26" s="12">
         <v>24</v>
@@ -3288,7 +3293,7 @@
         <v>94</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K26" s="13" t="s">
         <v>69</v>
@@ -3301,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P26" s="36" t="s">
         <v>19</v>
@@ -3316,7 +3321,7 @@
         <v>141</v>
       </c>
       <c r="T26" s="55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="U26" s="54" t="s">
         <v>143</v>
@@ -3336,11 +3341,11 @@
         <v>117</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H27" s="12">
         <v>25</v>
@@ -3349,7 +3354,7 @@
         <v>94</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>69</v>
@@ -3362,7 +3367,7 @@
         <v>24</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P27" s="36" t="s">
         <v>19</v>
@@ -3377,7 +3382,7 @@
         <v>141</v>
       </c>
       <c r="T27" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U27" s="54" t="s">
         <v>143</v>
@@ -3401,7 +3406,7 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H28" s="12">
         <v>26</v>
@@ -3423,7 +3428,7 @@
         <v>62</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P28" s="36" t="s">
         <v>19</v>
@@ -3438,7 +3443,7 @@
         <v>141</v>
       </c>
       <c r="T28" s="55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U28" s="54" t="s">
         <v>143</v>
@@ -3570,7 +3575,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H31" s="12">
         <v>29</v>
@@ -3579,7 +3584,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>69</v>
@@ -3605,7 +3610,7 @@
         <v>150</v>
       </c>
       <c r="T31" s="53" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U31" s="54" t="s">
         <v>151</v>
@@ -3681,7 +3686,7 @@
         <v>94</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>69</v>
@@ -3729,7 +3734,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H34" s="12">
         <v>32</v>
@@ -3738,7 +3743,7 @@
         <v>94</v>
       </c>
       <c r="J34" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>69</v>
@@ -3764,7 +3769,7 @@
         <v>141</v>
       </c>
       <c r="T34" s="55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="U34" s="54" t="s">
         <v>143</v>
@@ -3772,11 +3777,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3792,6 +3792,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de nombre rec110
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/ESCALETA_CN_08_01_CO.xlsx
@@ -523,9 +523,6 @@
     <t>En cada imagen se explica un tipo de neurona. Al hablar de las neuronas sensoriales debe explicar que estas hacen parte de los receptores, y que hay unos para estímulos internos y otros para estímulos externos. También que los nervios sensoriales se forman con agrupaciones de estas neuronas. En el segundo grupo, interneuronas, además de hablar de su función se debe aclarar que conforman el encéfalo y la médula espinal. Por último, al hablar de neuronas motoras se aclara que estas pueden estimular músculos o glándulas, y que conforman los nervios motores. Se debe explicar que a las neuronas sensoriales también se les llama aferentes, a las motoras eferentes y a las interneuronas se les dice neuronas de asociacón.</t>
   </si>
   <si>
-    <t>La transmisión de información entre células distintas</t>
-  </si>
-  <si>
     <t>Interactivo acerca de las células gliales</t>
   </si>
   <si>
@@ -749,6 +746,9 @@
   </si>
   <si>
     <t>Interactivo que trata sobre la plasticidad sináptica y su relación con los procesos cognitivos</t>
+  </si>
+  <si>
+    <t>La transmisión de información entre las células</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1932,7 @@
         <v>150</v>
       </c>
       <c r="T3" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U3" s="50" t="s">
         <v>151</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" s="12">
         <v>2</v>
@@ -1993,7 +1993,7 @@
         <v>141</v>
       </c>
       <c r="T4" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U4" s="54" t="s">
         <v>143</v>
@@ -2056,7 +2056,7 @@
         <v>150</v>
       </c>
       <c r="T5" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U5" s="54" t="s">
         <v>151</v>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="N6" s="15"/>
       <c r="O6" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P6" s="36" t="s">
         <v>19</v>
@@ -2119,7 +2119,7 @@
         <v>150</v>
       </c>
       <c r="T6" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U6" s="50" t="s">
         <v>151</v>
@@ -2145,7 +2145,7 @@
         <v>161</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H7" s="12">
         <v>5</v>
@@ -2154,7 +2154,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>69</v>
@@ -2243,7 +2243,7 @@
         <v>150</v>
       </c>
       <c r="T8" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U8" s="54" t="s">
         <v>151</v>
@@ -2269,7 +2269,7 @@
         <v>104</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H9" s="12">
         <v>7</v>
@@ -2278,7 +2278,7 @@
         <v>94</v>
       </c>
       <c r="J9" s="63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>69</v>
@@ -2291,7 +2291,7 @@
         <v>74</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P9" s="36" t="s">
         <v>20</v>
@@ -2332,7 +2332,7 @@
         <v>104</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H10" s="12">
         <v>8</v>
@@ -2341,7 +2341,7 @@
         <v>103</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>69</v>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="N10" s="15"/>
       <c r="O10" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P10" s="36" t="s">
         <v>19</v>
@@ -2369,7 +2369,7 @@
         <v>150</v>
       </c>
       <c r="T10" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U10" s="54" t="s">
         <v>151</v>
@@ -2395,7 +2395,7 @@
         <v>104</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H11" s="12">
         <v>9</v>
@@ -2404,7 +2404,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>69</v>
@@ -2417,7 +2417,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P11" s="36" t="s">
         <v>19</v>
@@ -2432,7 +2432,7 @@
         <v>141</v>
       </c>
       <c r="T11" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U11" s="54" t="s">
         <v>143</v>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="11" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="H12" s="12">
         <v>10</v>
@@ -2465,7 +2465,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>70</v>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H13" s="12">
         <v>11</v>
@@ -2522,7 +2522,7 @@
         <v>103</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>69</v>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="N13" s="15"/>
       <c r="O13" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P13" s="36" t="s">
         <v>19</v>
@@ -2583,7 +2583,7 @@
         <v>103</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K14" s="13" t="s">
         <v>69</v>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="N14" s="15"/>
       <c r="O14" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P14" s="36" t="s">
         <v>19</v>
@@ -2611,7 +2611,7 @@
         <v>150</v>
       </c>
       <c r="T14" s="58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U14" s="59" t="s">
         <v>151</v>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H15" s="12">
         <v>13</v>
@@ -2644,7 +2644,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>69</v>
@@ -2696,7 +2696,7 @@
         <v>104</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H16" s="12">
         <v>14</v>
@@ -2705,7 +2705,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>69</v>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H17" s="12">
         <v>15</v>
@@ -2764,7 +2764,7 @@
         <v>94</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>69</v>
@@ -2777,7 +2777,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P17" s="36" t="s">
         <v>19</v>
@@ -2792,7 +2792,7 @@
         <v>141</v>
       </c>
       <c r="T17" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U17" s="54" t="s">
         <v>143</v>
@@ -2809,12 +2809,12 @@
         <v>91</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="37"/>
       <c r="G18" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H18" s="12">
         <v>16</v>
@@ -2823,7 +2823,7 @@
         <v>103</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>69</v>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P18" s="36" t="s">
         <v>19</v>
@@ -2851,7 +2851,7 @@
         <v>150</v>
       </c>
       <c r="T18" s="55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U18" s="54" t="s">
         <v>151</v>
@@ -2868,12 +2868,12 @@
         <v>91</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="37"/>
       <c r="G19" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H19" s="12">
         <v>17</v>
@@ -2882,7 +2882,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>69</v>
@@ -2925,7 +2925,7 @@
         <v>91</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>109</v>
@@ -2982,7 +2982,7 @@
         <v>91</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>112</v>
@@ -3039,14 +3039,14 @@
         <v>91</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>99</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H22" s="12">
         <v>20</v>
@@ -3101,7 +3101,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H23" s="12">
         <v>21</v>
@@ -3110,7 +3110,7 @@
         <v>103</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K23" s="13" t="s">
         <v>69</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="N23" s="15"/>
       <c r="O23" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P23" s="36" t="s">
         <v>19</v>
@@ -3138,7 +3138,7 @@
         <v>150</v>
       </c>
       <c r="T23" s="55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U23" s="54" t="s">
         <v>151</v>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H24" s="12">
         <v>22</v>
@@ -3171,7 +3171,7 @@
         <v>94</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>69</v>
@@ -3184,10 +3184,10 @@
         <v>84</v>
       </c>
       <c r="O24" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="P24" s="36" t="s">
         <v>181</v>
-      </c>
-      <c r="P24" s="36" t="s">
-        <v>182</v>
       </c>
       <c r="Q24" s="51">
         <v>6</v>
@@ -3199,7 +3199,7 @@
         <v>141</v>
       </c>
       <c r="T24" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U24" s="54" t="s">
         <v>143</v>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H25" s="12">
         <v>23</v>
@@ -3232,7 +3232,7 @@
         <v>94</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>69</v>
@@ -3245,7 +3245,7 @@
         <v>77</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P25" s="36" t="s">
         <v>19</v>
@@ -3260,7 +3260,7 @@
         <v>141</v>
       </c>
       <c r="T25" s="55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U25" s="54" t="s">
         <v>143</v>
@@ -3284,7 +3284,7 @@
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H26" s="12">
         <v>24</v>
@@ -3293,7 +3293,7 @@
         <v>94</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K26" s="13" t="s">
         <v>69</v>
@@ -3306,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P26" s="36" t="s">
         <v>19</v>
@@ -3321,7 +3321,7 @@
         <v>141</v>
       </c>
       <c r="T26" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U26" s="54" t="s">
         <v>143</v>
@@ -3341,11 +3341,11 @@
         <v>117</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H27" s="12">
         <v>25</v>
@@ -3354,7 +3354,7 @@
         <v>94</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>69</v>
@@ -3367,7 +3367,7 @@
         <v>24</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P27" s="36" t="s">
         <v>19</v>
@@ -3382,7 +3382,7 @@
         <v>141</v>
       </c>
       <c r="T27" s="55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U27" s="54" t="s">
         <v>143</v>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H28" s="12">
         <v>26</v>
@@ -3428,7 +3428,7 @@
         <v>62</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P28" s="36" t="s">
         <v>19</v>
@@ -3443,7 +3443,7 @@
         <v>141</v>
       </c>
       <c r="T28" s="55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U28" s="54" t="s">
         <v>143</v>
@@ -3575,7 +3575,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H31" s="12">
         <v>29</v>
@@ -3584,7 +3584,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>69</v>
@@ -3610,7 +3610,7 @@
         <v>150</v>
       </c>
       <c r="T31" s="53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U31" s="54" t="s">
         <v>151</v>
@@ -3686,7 +3686,7 @@
         <v>94</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>69</v>
@@ -3734,7 +3734,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H34" s="12">
         <v>32</v>
@@ -3743,7 +3743,7 @@
         <v>94</v>
       </c>
       <c r="J34" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>69</v>
@@ -3769,7 +3769,7 @@
         <v>141</v>
       </c>
       <c r="T34" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U34" s="54" t="s">
         <v>143</v>

</xml_diff>